<commit_message>
Scarping Enhacements || Enhance the search function
</commit_message>
<xml_diff>
--- a/Results/London.xlsx
+++ b/Results/London.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,7 +424,7 @@
         <v>google</v>
       </c>
       <c r="B2" t="str">
-        <v>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiM5pnx6_yCAxWslVAGHe21DdwYABAAGgJkZw&amp;ase=2&amp;gclid=EAIaIQobChMIjOaZ8ev8ggMVrJVQBh3ttQ3cEBAYASAAEgI9mfD_BwE&amp;sig=AOD64_2EKxAFJXufZJ1VtAZUFp1O7xe7Pg&amp;adurl&amp;ctype=99</v>
+        <v>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwj8tZ3p7fyCAxWnZJEFHTGjCBUYABAAGgJscg&amp;ase=2&amp;gclid=EAIaIQobChMI_LWd6e38ggMVp2SRBR0xowgVEBAYASAAEgIJHfD_BwE&amp;sig=AOD64_1fMg5w2jnuxVVBjyMpP9pU9MCXmA&amp;adurl&amp;ctype=99&amp;nis=4&amp;ved=2ahUKEwiL5I_p7fyCAxUUGwYAHftOBE4Q8PwKegQIABAo</v>
       </c>
       <c r="C2" t="str">
         <v>London</v>
@@ -438,10 +438,10 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>google</v>
+        <v>makeagency</v>
       </c>
       <c r="B3" t="str">
-        <v>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiM5pnx6_yCAxWslVAGHe21DdwYABAHGgJkZw&amp;ase=2&amp;gclid=EAIaIQobChMIjOaZ8ev8ggMVrJVQBh3ttQ3cEBAYAiAAEgJaufD_BwE&amp;sig=AOD64_07pcM0tWGRBxQ0SXSd0zfAYcosgg&amp;adurl&amp;ctype=99</v>
+        <v>http://makeagency.co.uk/</v>
       </c>
       <c r="C3" t="str">
         <v>London</v>
@@ -450,7 +450,7 @@
         <v>UK</v>
       </c>
       <c r="E3" t="str">
-        <v>info@designinc.co.uk</v>
+        <v>hi@makeagency.co.uk</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>bartleboglehegarty</v>
+        <v>londonmarketingcompany</v>
       </c>
       <c r="B5" t="str">
-        <v>https://www.bartleboglehegarty.com/</v>
+        <v>http://www.londonmarketingcompany.co.uk/</v>
       </c>
       <c r="C5" t="str">
         <v>London</v>
@@ -484,15 +484,15 @@
         <v>UK</v>
       </c>
       <c r="E5" t="str">
-        <v>hello@bbh-usa.com, ellie.ring@bartleboglehegarty.com, andreas.bjork@bartleboglehegarty.com, sunayan.shahani@publicisgroupe.com, siying.goh@bartleboglehegarty.com</v>
+        <v>info@bathmarketingcompany.uixweb.dev</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>generationmedia</v>
+        <v>bartleboglehegarty</v>
       </c>
       <c r="B6" t="str">
-        <v>http://generationmedia.co.uk/</v>
+        <v>https://www.bartleboglehegarty.com/</v>
       </c>
       <c r="C6" t="str">
         <v>London</v>
@@ -501,15 +501,15 @@
         <v>UK</v>
       </c>
       <c r="E6" t="str">
-        <v>contact@generationmedia.co.uk</v>
+        <v>hello@bbh-usa.com, ellie.ring@bartleboglehegarty.com, andreas.bjork@bartleboglehegarty.com, sunayan.shahani@publicisgroupe.com, siying.goh@bartleboglehegarty.com</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>saatchi</v>
+        <v>generationmedia</v>
       </c>
       <c r="B7" t="str">
-        <v>https://saatchi.co.uk/</v>
+        <v>http://generationmedia.co.uk/</v>
       </c>
       <c r="C7" t="str">
         <v>London</v>
@@ -518,15 +518,15 @@
         <v>UK</v>
       </c>
       <c r="E7" t="str">
-        <v>hello@saatchi.co.uk, talent@saatchi.co.uk</v>
+        <v>contact@generationmedia.co.uk</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>vccp</v>
+        <v>saatchi</v>
       </c>
       <c r="B8" t="str">
-        <v>http://www.vccp.com/</v>
+        <v>https://saatchi.co.uk/</v>
       </c>
       <c r="C8" t="str">
         <v>London</v>
@@ -535,15 +535,15 @@
         <v>UK</v>
       </c>
       <c r="E8" t="str">
-        <v>info@vccp.com, stephanieb@vccp.com, gwright@vccp.com, joinus@vccp.com</v>
+        <v>hello@saatchi.co.uk, talent@saatchi.co.uk</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>ality</v>
+        <v>unrvld</v>
       </c>
       <c r="B9" t="str">
-        <v>https://www.ality.co.uk/</v>
+        <v>https://unrvld.com/</v>
       </c>
       <c r="C9" t="str">
         <v>London</v>
@@ -552,15 +552,15 @@
         <v>UK</v>
       </c>
       <c r="E9" t="str">
-        <v>hello@ality.co.uk</v>
+        <v>hello@unrvld.com, marketing@unrvld.com, vacancies@unrvld.com</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>hexdigital</v>
+        <v>vccp</v>
       </c>
       <c r="B10" t="str">
-        <v>https://hexdigital.com/</v>
+        <v>http://www.vccp.com/</v>
       </c>
       <c r="C10" t="str">
         <v>London</v>
@@ -569,15 +569,15 @@
         <v>UK</v>
       </c>
       <c r="E10" t="str">
-        <v>hello@hexdigital.com</v>
+        <v>info@vccp.com, stephanieb@vccp.com, gwright@vccp.com, joinus@vccp.com</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>minttwist</v>
+        <v>ality</v>
       </c>
       <c r="B11" t="str">
-        <v>https://www.minttwist.com/</v>
+        <v>https://www.ality.co.uk/</v>
       </c>
       <c r="C11" t="str">
         <v>London</v>
@@ -586,15 +586,15 @@
         <v>UK</v>
       </c>
       <c r="E11" t="str">
-        <v>hello@minttwist.com</v>
+        <v>hello@ality.co.uk</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>cardellmedia</v>
+        <v>hexdigital</v>
       </c>
       <c r="B12" t="str">
-        <v>https://www.cardellmedia.com/</v>
+        <v>https://hexdigital.com/</v>
       </c>
       <c r="C12" t="str">
         <v>London</v>
@@ -603,15 +603,15 @@
         <v>UK</v>
       </c>
       <c r="E12" t="str">
-        <v>support@cardellmedia.com</v>
+        <v>hello@hexdigital.com</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>weareroast</v>
+        <v>minttwist</v>
       </c>
       <c r="B13" t="str">
-        <v>https://weareroast.com/</v>
+        <v>https://www.minttwist.com/</v>
       </c>
       <c r="C13" t="str">
         <v>London</v>
@@ -620,29 +620,63 @@
         <v>UK</v>
       </c>
       <c r="E13" t="str">
-        <v>roast@tipigroup.com</v>
+        <v>hello@minttwist.com</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
+        <v>cardellmedia</v>
+      </c>
+      <c r="B14" t="str">
+        <v>https://www.cardellmedia.com/</v>
+      </c>
+      <c r="C14" t="str">
+        <v>London</v>
+      </c>
+      <c r="D14" t="str">
+        <v>UK</v>
+      </c>
+      <c r="E14" t="str">
+        <v>support@cardellmedia.com</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>weareroast</v>
+      </c>
+      <c r="B15" t="str">
+        <v>https://weareroast.com/</v>
+      </c>
+      <c r="C15" t="str">
+        <v>London</v>
+      </c>
+      <c r="D15" t="str">
+        <v>UK</v>
+      </c>
+      <c r="E15" t="str">
+        <v>roast@tipigroup.com</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
         <v>iseemedia</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B16" t="str">
         <v>http://www.iseemedia.net/</v>
       </c>
-      <c r="C14" t="str">
-        <v>London</v>
-      </c>
-      <c r="D14" t="str">
-        <v>UK</v>
-      </c>
-      <c r="E14" t="str">
+      <c r="C16" t="str">
+        <v>London</v>
+      </c>
+      <c r="D16" t="str">
+        <v>UK</v>
+      </c>
+      <c r="E16" t="str">
         <v>info@iseemedia.net</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scarping Enhacements || navigateWithRetry func
</commit_message>
<xml_diff>
--- a/Results/London.xlsx
+++ b/Results/London.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,7 +424,7 @@
         <v>google</v>
       </c>
       <c r="B2" t="str">
-        <v>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwj8tZ3p7fyCAxWnZJEFHTGjCBUYABAAGgJscg&amp;ase=2&amp;gclid=EAIaIQobChMI_LWd6e38ggMVp2SRBR0xowgVEBAYASAAEgIJHfD_BwE&amp;sig=AOD64_1fMg5w2jnuxVVBjyMpP9pU9MCXmA&amp;adurl&amp;ctype=99&amp;nis=4&amp;ved=2ahUKEwiL5I_p7fyCAxUUGwYAHftOBE4Q8PwKegQIABAo</v>
+        <v>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjhw_eAgP2CAxWVXpEFHfP2DxEYABAAGgJscg&amp;ase=2&amp;gclid=EAIaIQobChMI4cP3gID9ggMVlV6RBR3z9g8REBAYASAAEgLelPD_BwE&amp;sig=AOD64_3N2VaRGe2qXXt-6MBEf3xs6xeQMw&amp;adurl&amp;ctype=99</v>
       </c>
       <c r="C2" t="str">
         <v>London</v>
@@ -455,10 +455,10 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>you-agency</v>
+        <v>sidedishmedia</v>
       </c>
       <c r="B4" t="str">
-        <v>http://www.you-agency.com/</v>
+        <v>https://www.sidedishmedia.co.uk/</v>
       </c>
       <c r="C4" t="str">
         <v>London</v>
@@ -467,15 +467,15 @@
         <v>UK</v>
       </c>
       <c r="E4" t="str">
-        <v>hello@you-agency.com</v>
+        <v>hello@sidedishmedia.co.uk</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>londonmarketingcompany</v>
+        <v>you-agency</v>
       </c>
       <c r="B5" t="str">
-        <v>http://www.londonmarketingcompany.co.uk/</v>
+        <v>http://www.you-agency.com/</v>
       </c>
       <c r="C5" t="str">
         <v>London</v>
@@ -484,15 +484,15 @@
         <v>UK</v>
       </c>
       <c r="E5" t="str">
-        <v>info@bathmarketingcompany.uixweb.dev</v>
+        <v>hello@you-agency.com</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>bartleboglehegarty</v>
+        <v>londonmarketingcompany</v>
       </c>
       <c r="B6" t="str">
-        <v>https://www.bartleboglehegarty.com/</v>
+        <v>http://www.londonmarketingcompany.co.uk/</v>
       </c>
       <c r="C6" t="str">
         <v>London</v>
@@ -501,15 +501,15 @@
         <v>UK</v>
       </c>
       <c r="E6" t="str">
-        <v>hello@bbh-usa.com, ellie.ring@bartleboglehegarty.com, andreas.bjork@bartleboglehegarty.com, sunayan.shahani@publicisgroupe.com, siying.goh@bartleboglehegarty.com</v>
+        <v>info@bathmarketingcompany.uixweb.dev</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>generationmedia</v>
+        <v>bartleboglehegarty</v>
       </c>
       <c r="B7" t="str">
-        <v>http://generationmedia.co.uk/</v>
+        <v>https://www.bartleboglehegarty.com/</v>
       </c>
       <c r="C7" t="str">
         <v>London</v>
@@ -518,15 +518,15 @@
         <v>UK</v>
       </c>
       <c r="E7" t="str">
-        <v>contact@generationmedia.co.uk</v>
+        <v>hello@bbh-usa.com, ellie.ring@bartleboglehegarty.com, andreas.bjork@bartleboglehegarty.com, sunayan.shahani@publicisgroupe.com, siying.goh@bartleboglehegarty.com</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>saatchi</v>
+        <v>generationmedia</v>
       </c>
       <c r="B8" t="str">
-        <v>https://saatchi.co.uk/</v>
+        <v>http://generationmedia.co.uk/</v>
       </c>
       <c r="C8" t="str">
         <v>London</v>
@@ -535,15 +535,15 @@
         <v>UK</v>
       </c>
       <c r="E8" t="str">
-        <v>hello@saatchi.co.uk, talent@saatchi.co.uk</v>
+        <v>contact@generationmedia.co.uk</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>unrvld</v>
+        <v>saatchi</v>
       </c>
       <c r="B9" t="str">
-        <v>https://unrvld.com/</v>
+        <v>https://saatchi.co.uk/</v>
       </c>
       <c r="C9" t="str">
         <v>London</v>
@@ -552,15 +552,15 @@
         <v>UK</v>
       </c>
       <c r="E9" t="str">
-        <v>hello@unrvld.com, marketing@unrvld.com, vacancies@unrvld.com</v>
+        <v>hello@saatchi.co.uk, talent@saatchi.co.uk</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>vccp</v>
+        <v>unrvld</v>
       </c>
       <c r="B10" t="str">
-        <v>http://www.vccp.com/</v>
+        <v>https://unrvld.com/</v>
       </c>
       <c r="C10" t="str">
         <v>London</v>
@@ -569,15 +569,15 @@
         <v>UK</v>
       </c>
       <c r="E10" t="str">
-        <v>info@vccp.com, stephanieb@vccp.com, gwright@vccp.com, joinus@vccp.com</v>
+        <v>hello@unrvld.com, marketing@unrvld.com, vacancies@unrvld.com</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>ality</v>
+        <v>vccp</v>
       </c>
       <c r="B11" t="str">
-        <v>https://www.ality.co.uk/</v>
+        <v>http://www.vccp.com/</v>
       </c>
       <c r="C11" t="str">
         <v>London</v>
@@ -586,15 +586,15 @@
         <v>UK</v>
       </c>
       <c r="E11" t="str">
-        <v>hello@ality.co.uk</v>
+        <v>info@vccp.com, stephanieb@vccp.com, gwright@vccp.com, joinus@vccp.com</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>hexdigital</v>
+        <v>ality</v>
       </c>
       <c r="B12" t="str">
-        <v>https://hexdigital.com/</v>
+        <v>https://www.ality.co.uk/</v>
       </c>
       <c r="C12" t="str">
         <v>London</v>
@@ -603,15 +603,15 @@
         <v>UK</v>
       </c>
       <c r="E12" t="str">
-        <v>hello@hexdigital.com</v>
+        <v>hello@ality.co.uk</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>minttwist</v>
+        <v>hexdigital</v>
       </c>
       <c r="B13" t="str">
-        <v>https://www.minttwist.com/</v>
+        <v>https://hexdigital.com/</v>
       </c>
       <c r="C13" t="str">
         <v>London</v>
@@ -620,15 +620,15 @@
         <v>UK</v>
       </c>
       <c r="E13" t="str">
-        <v>hello@minttwist.com</v>
+        <v>hello@hexdigital.com</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>cardellmedia</v>
+        <v>minttwist</v>
       </c>
       <c r="B14" t="str">
-        <v>https://www.cardellmedia.com/</v>
+        <v>https://www.minttwist.com/</v>
       </c>
       <c r="C14" t="str">
         <v>London</v>
@@ -637,15 +637,15 @@
         <v>UK</v>
       </c>
       <c r="E14" t="str">
-        <v>support@cardellmedia.com</v>
+        <v>hello@minttwist.com</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>weareroast</v>
+        <v>cardellmedia</v>
       </c>
       <c r="B15" t="str">
-        <v>https://weareroast.com/</v>
+        <v>https://www.cardellmedia.com/</v>
       </c>
       <c r="C15" t="str">
         <v>London</v>
@@ -654,29 +654,46 @@
         <v>UK</v>
       </c>
       <c r="E15" t="str">
-        <v>roast@tipigroup.com</v>
+        <v>support@cardellmedia.com</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
+        <v>weareroast</v>
+      </c>
+      <c r="B16" t="str">
+        <v>https://weareroast.com/</v>
+      </c>
+      <c r="C16" t="str">
+        <v>London</v>
+      </c>
+      <c r="D16" t="str">
+        <v>UK</v>
+      </c>
+      <c r="E16" t="str">
+        <v>roast@tipigroup.com</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
         <v>iseemedia</v>
       </c>
-      <c r="B16" t="str">
+      <c r="B17" t="str">
         <v>http://www.iseemedia.net/</v>
       </c>
-      <c r="C16" t="str">
-        <v>London</v>
-      </c>
-      <c r="D16" t="str">
-        <v>UK</v>
-      </c>
-      <c r="E16" t="str">
+      <c r="C17" t="str">
+        <v>London</v>
+      </c>
+      <c r="D17" t="str">
+        <v>UK</v>
+      </c>
+      <c r="E17" t="str">
         <v>info@iseemedia.net</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scarping Enhacements || Extracting the agency Name
</commit_message>
<xml_diff>
--- a/Results/London.xlsx
+++ b/Results/London.xlsx
@@ -421,10 +421,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>google</v>
+        <v>oneday</v>
       </c>
       <c r="B2" t="str">
-        <v>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjhw_eAgP2CAxWVXpEFHfP2DxEYABAAGgJscg&amp;ase=2&amp;gclid=EAIaIQobChMI4cP3gID9ggMVlV6RBR3z9g8REBAYASAAEgLelPD_BwE&amp;sig=AOD64_3N2VaRGe2qXXt-6MBEf3xs6xeQMw&amp;adurl&amp;ctype=99</v>
+        <v>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwi8nNbXgv2CAxWykmgJHTOCDG0YABAAGgJ3Zg&amp;ase=2&amp;gclid=EAIaIQobChMIvJzW14L9ggMVspJoCR0zggxtEBAYASAAEgJAHvD_BwE&amp;sig=AOD64_2E9U-QK_qGM4hW0cWuw4HufTXQRQ&amp;adurl&amp;ctype=99</v>
       </c>
       <c r="C2" t="str">
         <v>London</v>
@@ -438,7 +438,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>makeagency</v>
+        <v>makeagency.co</v>
       </c>
       <c r="B3" t="str">
         <v>http://makeagency.co.uk/</v>
@@ -455,7 +455,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>sidedishmedia</v>
+        <v>sidedishmedia.co</v>
       </c>
       <c r="B4" t="str">
         <v>https://www.sidedishmedia.co.uk/</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>londonmarketingcompany</v>
+        <v>bathmarketingcompany.uixweb</v>
       </c>
       <c r="B6" t="str">
         <v>http://www.londonmarketingcompany.co.uk/</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>bartleboglehegarty</v>
+        <v>bbh-usa</v>
       </c>
       <c r="B7" t="str">
         <v>https://www.bartleboglehegarty.com/</v>
@@ -523,7 +523,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>generationmedia</v>
+        <v>generationmedia.co</v>
       </c>
       <c r="B8" t="str">
         <v>http://generationmedia.co.uk/</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>saatchi</v>
+        <v>saatchi.co</v>
       </c>
       <c r="B9" t="str">
         <v>https://saatchi.co.uk/</v>
@@ -591,7 +591,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>ality</v>
+        <v>ality.co</v>
       </c>
       <c r="B12" t="str">
         <v>https://www.ality.co.uk/</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>weareroast</v>
+        <v>tipigroup</v>
       </c>
       <c r="B16" t="str">
         <v>https://weareroast.com/</v>

</xml_diff>